<commit_message>
шефы + readme hotfix
</commit_message>
<xml_diff>
--- a/Шефы.xlsx
+++ b/Шефы.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrey\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Учеба\Уник\Младшим\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="23040" windowHeight="9372" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="351003" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>№</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>vk шефов</t>
+  </si>
+  <si>
+    <t>https://vk.com/d.gallavich</t>
   </si>
 </sst>
 </file>
@@ -392,9 +395,6 @@
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -419,9 +419,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -443,6 +440,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -725,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,236 +741,240 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+      <c r="A1" s="26">
         <v>351003</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="6"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="6"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="6"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="6"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="6"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="6"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="6"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="6"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="6"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="6"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -981,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,360 +1001,360 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16">
+      <c r="A1" s="27">
         <v>351004</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="18">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="18">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="18">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18">
+      <c r="A6" s="16">
         <v>4</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="6"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="18">
+      <c r="A7" s="16">
         <v>5</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="6"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="18">
+      <c r="A8" s="16">
         <v>6</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="18">
+      <c r="A9" s="16">
         <v>7</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="18">
+      <c r="A10" s="16">
         <v>8</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="6"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18">
+      <c r="A11" s="16">
         <v>9</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="6"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="18">
+      <c r="A12" s="16">
         <v>10</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="18">
+      <c r="A13" s="16">
         <v>11</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="6"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="18">
+      <c r="A14" s="16">
         <v>12</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="6"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18">
+      <c r="A15" s="16">
         <v>13</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="6"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="18">
+      <c r="A16" s="16">
         <v>14</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="6"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="18">
+      <c r="A17" s="16">
         <v>15</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="6"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18">
+      <c r="A18" s="16">
         <v>16</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="6"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="18">
+      <c r="A19" s="16">
         <v>17</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="6"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="18">
+      <c r="A20" s="16">
         <v>18</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="6"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="18">
+      <c r="A21" s="16">
         <v>19</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="6"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="18">
+      <c r="A22" s="16">
         <v>20</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="6"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="18">
+      <c r="A23" s="16">
         <v>21</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="6"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="18">
+      <c r="A24" s="16">
         <v>22</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="6"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="18">
+      <c r="A25" s="16">
         <v>23</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="6"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="18">
+      <c r="A26" s="16">
         <v>24</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="6"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="18">
+      <c r="A27" s="16">
         <v>25</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="6"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="18">
+      <c r="A28" s="16">
         <v>26</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="6"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="18">
+      <c r="A29" s="16">
         <v>27</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="6"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="18">
+      <c r="A30" s="16">
         <v>28</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="6"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="18">
+      <c r="A31" s="16">
         <v>29</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="6"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="24">
+      <c r="A32" s="22">
         <v>30</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="9"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>